<commit_message>
Changes in Data Utils
</commit_message>
<xml_diff>
--- a/exam_timetable.xlsx
+++ b/exam_timetable.xlsx
@@ -463,20 +463,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VLS 804</t>
+          <t>DHS 101B-B</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>09:15 - 12:15</t>
+          <t>09:45 - 12:45</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Ramanujan Basement 05 (E- Block) (Capacity: 31.0)</t>
+          <t>R106 (LAB) (Capacity: 8.0), R107/R108 (LAB) (Capacity: 115.0)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -488,20 +488,20 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CSE 836</t>
+          <t>DHS 315</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>09:45 - 12:45</t>
+          <t>10:45 - 12:45</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R104 (Capacity: 14.0)</t>
+          <t>R203 (Capacity: 78.0)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -513,20 +513,20 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CSE 718</t>
+          <t>CSE 816</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>41</v>
+        <v>146</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>09:45 - 12:45</t>
+          <t>10:45 - 12:45</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>R103 (Capacity: 41.0)</t>
+          <t>R103 (Capacity: 146.0)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -538,7 +538,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DAS 101P-A</t>
+          <t>DAS 101-A</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -546,12 +546,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>09:45 - 12:15</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R107/R108 (LAB) (Capacity: 96.0)</t>
+          <t>R203 (Capacity: 96.0)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -563,20 +563,20 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AIM 843</t>
+          <t>AIM 845</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>10:45 - 11:45</t>
+          <t>14:15 - 17:15</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>A310 (Capacity: 35.0)</t>
+          <t>R102 (Capacity: 7.0)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -588,7 +588,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>EGC 123-B</t>
+          <t>DAS 101-B</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -596,12 +596,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>10:45 - 12:45</t>
+          <t>14:15 - 17:15</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>A106 (Capacity: 95.0)</t>
+          <t>A307 (Capacity: 95.0)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -613,20 +613,20 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DHS 305</t>
+          <t>DHS 201-A</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>36</v>
+        <v>158</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>14:15 - 16:15</t>
+          <t>14:45 - 17:45</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>A303 (Capacity: 36.0)</t>
+          <t>R103 (Capacity: 158.0)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -638,20 +638,20 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DAS 101P-B</t>
+          <t>ECE 212P</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>14:15 - 16:45</t>
+          <t>15:00 - 18:00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>R107/R108 (LAB) (Capacity: 95.0)</t>
+          <t>A317 HidesLab (Capacity: 61.0)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -663,20 +663,20 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ECE 212P</t>
+          <t>CSE 102 P-A</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>61</v>
+        <v>158</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>15:00 - 18:00</t>
+          <t>15:00 - 17:30</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>A317 HidesLab (Capacity: 61.0)</t>
+          <t>R401(Amanthran) (Capacity: 158.0)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -688,45 +688,45 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CSE 102 P-A</t>
+          <t>AMS 403</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>158</v>
+        <v>79</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>15:15 - 17:45</t>
+          <t>09:30 - 12:00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>A106 (Capacity: 158.0)</t>
+          <t>Ramanujan Basement 04 (D- Block) (Capacity: 79.0)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Tue</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>AMS 401</t>
+          <t>AMS 404</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>09:15 - 12:15</t>
+          <t>10:30 - 12:30</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Ramanujan Basement 01 (A- Block) (Capacity: 4.0)</t>
+          <t>Ramanujan Basement 03 (C- Block) (Capacity: 75.0)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -738,20 +738,20 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>DHS 611</t>
+          <t>EGC 123-B</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>09:15 - 12:15</t>
+          <t>10:45 - 12:45</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>A303 (Capacity: 12.0)</t>
+          <t>R103 (Capacity: 95.0)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -763,20 +763,20 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>DHS 201-B</t>
+          <t>CSE 606</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>123</v>
+        <v>14</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>09:15 - 12:15</t>
+          <t>11:30 - 13:00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>R103 (Capacity: 123.0)</t>
+          <t>A304/A305 (Capacity: 14.0)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -788,20 +788,20 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>DHS 315</t>
+          <t>AMS 401</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>09:30 - 11:30</t>
+          <t>14:15 - 17:15</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>A304/A305 (Capacity: 78.0)</t>
+          <t>R104 (Capacity: 4.0)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -813,20 +813,20 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>AMS 403</t>
+          <t>AIM 102</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>10:15 - 12:45</t>
+          <t>14:15 - 17:15</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>A204 (Capacity: 79.0)</t>
+          <t>R102 (Capacity: 59.0)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -838,20 +838,20 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CSE 816</t>
+          <t>DHS 611</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>146</v>
+        <v>12</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>10:30 - 12:30</t>
+          <t>14:45 - 17:45</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>R401(Amanthran) (Capacity: 146.0)</t>
+          <t>R101 (Capacity: 12.0)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -863,20 +863,20 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>AMS 404</t>
+          <t>CSE 704</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>10:45 - 12:45</t>
+          <t>14:45 - 17:15</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Ramanujan Basement 05 (E- Block) (Capacity: 75.0)</t>
+          <t>R401(Amanthran) (Capacity: 115.0)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -888,20 +888,20 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>COM 605</t>
+          <t>VLS 603</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>15:00 - 18:00</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>R104 (Capacity: 12.0)</t>
+          <t>A307 (Capacity: 33.0)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -913,20 +913,20 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AIM 821</t>
+          <t>AMS 402</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>15:00 - 18:00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>A307 (Capacity: 21.0)</t>
+          <t>R110 (Capacity: 39.0)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -938,20 +938,20 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>AMS 402</t>
+          <t>DHS 308</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>15:00 - 18:00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>A106 (Capacity: 39.0)</t>
+          <t>A304/A305 (Capacity: 40.0)</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -963,20 +963,20 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>AIM 845</t>
+          <t>DHS 101B-A</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>14:15 - 17:15</t>
+          <t>15:00 - 18:00</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>R105 (Capacity: 7.0)</t>
+          <t>R106 (LAB) (Capacity: 43.0), R107/R108 (LAB) (Capacity: 115.0)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -988,70 +988,70 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CSE 102-A</t>
+          <t>CSE 104-A</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>15:00 - 18:00</t>
+          <t>09:15 - 11:15</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>R103 (Capacity: 159.0)</t>
+          <t>R203 (Capacity: 158.0)</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Tue</t>
+          <t>Wed</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>AIM 101</t>
+          <t>DHS 314</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>15:15 - 17:15</t>
+          <t>10:45 - 12:45</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>R101 (Capacity: 59.0)</t>
+          <t>R103 (Capacity: 25.0)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Tue</t>
+          <t>Wed</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CSE 104-A</t>
+          <t>AIM 101</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>158</v>
+        <v>59</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>09:15 - 11:15</t>
+          <t>10:45 - 12:45</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>A106 (Capacity: 158.0)</t>
+          <t>R101 (Capacity: 59.0)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1063,20 +1063,20 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>EGC 301</t>
+          <t>DAS 839</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>193</v>
+        <v>72</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>09:15 - 12:15</t>
+          <t>10:45 - 12:45</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>R203 (Capacity: 193.0)</t>
+          <t>Ramanujan Basement 01 (A- Block) (Capacity: 72.0)</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1088,20 +1088,20 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CSE 102-B</t>
+          <t>ECE 304</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>123</v>
+        <v>61</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>09:30 - 11:30</t>
+          <t>11:30 - 13:00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>R401(Amanthran) (Capacity: 123.0)</t>
+          <t>Ramanujan Basement 03 (C- Block) (Capacity: 61.0)</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1113,20 +1113,20 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>AIM 831</t>
+          <t>EGC 301</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>09:45 - 12:45</t>
+          <t>14:15 - 17:15</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>R106 (LAB) (Capacity: 70.0), R107/R108 (LAB) (Capacity: 105.0)</t>
+          <t>A106 (Capacity: 193.0)</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1138,20 +1138,20 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>DAS 839</t>
+          <t>CSE 102 P-B</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>72</v>
+        <v>123</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>15:00 - 17:30</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Ramanujan Basement 05 (E- Block) (Capacity: 72.0)</t>
+          <t>R203 (Capacity: 123.0)</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1163,20 +1163,20 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CSE 104-B</t>
+          <t>AIM 831</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>123</v>
+        <v>175</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>15:00 - 18:00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>R203 (Capacity: 123.0)</t>
+          <t>R106 (LAB) (Capacity: 70.0), R107/R108 (LAB) (Capacity: 105.0)</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1188,36 +1188,36 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>DHS 314</t>
+          <t>VLS 804</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>15:45 - 17:45</t>
+          <t>09:45 - 12:45</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>R102 (Capacity: 25.0)</t>
+          <t>Ramanujan Basement 04 (D- Block) (Capacity: 31.0)</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Thu</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CSE 754</t>
+          <t>ECE 303P</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Ramanujan Basement 02 (B- Block) (Capacity: 25.0)</t>
+          <t>A317 HidesLab (Capacity: 61.0)</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1238,11 +1238,11 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>DHS 308</t>
+          <t>CSE 104-B</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>40</v>
+        <v>123</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Ramanujan Basement 05 (E- Block) (Capacity: 40.0)</t>
+          <t>R103 (Capacity: 123.0)</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1263,20 +1263,20 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ECE 303P</t>
+          <t>DAS 605</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>09:45 - 12:45</t>
+          <t>10:45 - 12:45</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>A317 HidesLab (Capacity: 61.0)</t>
+          <t>R102 (Capacity: 53.0)</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1288,20 +1288,20 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>DHS 101B-A</t>
+          <t>CSE 212</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>09:45 - 12:45</t>
+          <t>10:45 - 12:45</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>R106 (LAB) (Capacity: 44.0), R107/R108 (LAB) (Capacity: 114.0)</t>
+          <t>R203 (Capacity: 134.0)</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1313,20 +1313,20 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CSE 102 P-B</t>
+          <t>DHS 306</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>123</v>
+        <v>34</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>10:30 - 13:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>R401(Amanthran) (Capacity: 123.0)</t>
+          <t>R203 (Capacity: 34.0)</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1338,20 +1338,20 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>CSE 212</t>
+          <t>AIM 832</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>134</v>
+        <v>93</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>10:45 - 12:45</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>R203 (Capacity: 134.0)</t>
+          <t>R401(Amanthran) (Capacity: 93.0)</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1363,7 +1363,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ECE 304</t>
+          <t>ECE 212</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1371,12 +1371,12 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>14:00 - 15:30</t>
+          <t>14:15 - 17:15</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>A204 (Capacity: 61.0)</t>
+          <t>R103 (Capacity: 61.0)</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1388,20 +1388,20 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>AIM 832</t>
+          <t>AIM 821</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>93</v>
+        <v>21</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>14:15 - 17:15</t>
+          <t>15:00 - 18:00</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>R103 (Capacity: 93.0)</t>
+          <t>R105 (Capacity: 21.0)</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1413,20 +1413,20 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>EGC 123-A</t>
+          <t>EGC 121-B</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>15:00 - 17:00</t>
+          <t>15:00 - 18:00</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>R203 (Capacity: 127.0)</t>
+          <t>A106 (Capacity: 95.0)</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1438,36 +1438,36 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>DHS 101B-B</t>
+          <t>EGC 123-A</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>09:15 - 12:15</t>
+          <t>15:00 - 17:00</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>R106 (LAB) (Capacity: 70.0), R107/R108 (LAB) (Capacity: 53.0)</t>
+          <t>R203 (Capacity: 127.0)</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Thu</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>DHS 201-A</t>
+          <t>CSE 754</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>158</v>
+        <v>25</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1476,7 +1476,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>A106 (Capacity: 158.0)</t>
+          <t>R105 (Capacity: 25.0)</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1488,20 +1488,20 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>CSE 824</t>
+          <t>AIM 846</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>155</v>
+        <v>26</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>09:30 - 12:30</t>
+          <t>09:45 - 12:45</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>R103 (Capacity: 155.0)</t>
+          <t>Ramanujan Basement 05 (E- Block) (Capacity: 26.0)</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1513,7 +1513,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ECE 212</t>
+          <t>ECE 303</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1521,12 +1521,12 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>09:45 - 12:45</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>R103 (Capacity: 61.0)</t>
+          <t>Ramanujan Basement 02 (B- Block) (Capacity: 61.0)</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>DAS 101-B</t>
+          <t>DAS 101P-B</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1546,12 +1546,12 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>10:15 - 12:45</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>A106 (Capacity: 95.0)</t>
+          <t>R107/R108 (LAB) (Capacity: 95.0)</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1563,20 +1563,20 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>DHS 108</t>
+          <t>DHS 305</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>14:15 - 17:15</t>
+          <t>10:45 - 12:45</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Ramanujan Basement 03 (C- Block) (Capacity: 7.0)</t>
+          <t>R104 (Capacity: 36.0)</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1588,20 +1588,20 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>AIM 846</t>
+          <t>AIM 704</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>14:15 - 17:15</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>R104 (Capacity: 26.0)</t>
+          <t>R110 (Capacity: 20.0)</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1613,20 +1613,20 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>DAS 101-A</t>
+          <t>AIM 843</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>14:45 - 17:45</t>
+          <t>14:00 - 15:00</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>R203 (Capacity: 96.0)</t>
+          <t>R103 (Capacity: 35.0)</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1638,145 +1638,145 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>AIM 704</t>
+          <t>DAS 101P-A</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>09:30 - 12:30</t>
+          <t>14:00 - 16:30</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>R102 (Capacity: 20.0)</t>
+          <t>R107/R108 (LAB) (Capacity: 96.0)</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Fri</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>DAS 605</t>
+          <t>CSE 836</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>09:30 - 11:30</t>
+          <t>14:15 - 17:15</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>A304/A305 (Capacity: 53.0)</t>
+          <t>R104 (Capacity: 14.0)</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Fri</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>ECE 303</t>
+          <t>CSE 718</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>09:45 - 12:45</t>
+          <t>15:00 - 18:00</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>R105 (Capacity: 61.0)</t>
+          <t>R110 (Capacity: 41.0)</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Fri</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>CSE 606</t>
+          <t>DHS 201-A</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>14</v>
+        <v>158</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11:30 - 13:00</t>
+          <t>15:00 - 18:00</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>R101 (Capacity: 14.0)</t>
+          <t>R401(Amanthran) (Capacity: 158.0)</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Fri</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>DHS 306</t>
+          <t>CSE 102-B</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>34</v>
+        <v>123</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>15:45 - 17:45</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Ramanujan Basement 03 (C- Block) (Capacity: 34.0)</t>
+          <t>R203 (Capacity: 123.0)</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Fri</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>AIM 102</t>
+          <t>CSE 102-A</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>09:30 - 12:30</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>A303 (Capacity: 59.0)</t>
+          <t>A106 (Capacity: 159.0)</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -1788,20 +1788,20 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>EGC 121-B</t>
+          <t>CSE 824</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>95</v>
+        <v>155</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>09:45 - 12:45</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>A204 (Capacity: 95.0)</t>
+          <t>R203 (Capacity: 155.0)</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1813,20 +1813,20 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>DHS 110</t>
+          <t>DHS 108</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>193</v>
+        <v>7</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>A106 (Capacity: 193.0)</t>
+          <t>R105 (Capacity: 7.0)</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1838,20 +1838,20 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>EGC 121-A</t>
+          <t>DHS 201-B</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>14:15 - 17:15</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>R203 (Capacity: 127.0)</t>
+          <t>R103 (Capacity: 123.0)</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -1863,20 +1863,20 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>DHS 201-A</t>
+          <t>EGC 121-A</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>14:15 - 17:15</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>R401(Amanthran) (Capacity: 158.0)</t>
+          <t>R203 (Capacity: 127.0)</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -1888,20 +1888,20 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>VLS 603</t>
+          <t>DHS 110</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>33</v>
+        <v>193</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>14:45 - 17:45</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>R102 (Capacity: 33.0)</t>
+          <t>A106 (Capacity: 193.0)</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -1913,20 +1913,20 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>CSE 704</t>
+          <t>COM 605</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>15:00 - 17:30</t>
+          <t>15:00 - 17:00</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>R103 (Capacity: 115.0)</t>
+          <t>R102 (Capacity: 12.0)</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">

</xml_diff>